<commit_message>
Added Conclusion and updated data sort page
</commit_message>
<xml_diff>
--- a/LCFC_Game_Data.xlsx
+++ b/LCFC_Game_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="2600" windowWidth="25600" windowHeight="20720" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -163,6 +163,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -217,7 +220,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -225,7 +228,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -563,13 +569,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="2" customWidth="1"/>
+    <col min="1" max="1" width="12.5" style="4" customWidth="1"/>
     <col min="2" max="2" width="19.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.83203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" style="2" customWidth="1"/>
@@ -580,7 +586,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -609,7 +615,7 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="3">
+      <c r="A2" s="4">
         <v>42819</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -638,7 +644,7 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="3">
+      <c r="A3" s="4">
         <v>42824</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -667,7 +673,7 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="3">
+      <c r="A4" s="4">
         <v>42833</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -696,7 +702,7 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="3">
+      <c r="A5" s="4">
         <v>42840</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -725,7 +731,7 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="3">
+      <c r="A6" s="4">
         <v>42847</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -754,7 +760,7 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="3">
+      <c r="A7" s="4">
         <v>42854</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -783,7 +789,7 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="3">
+      <c r="A8" s="4">
         <v>42868</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -812,7 +818,7 @@
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="3">
+      <c r="A9" s="4">
         <v>42875</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -841,7 +847,7 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="3">
+      <c r="A10" s="4">
         <v>42889</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -870,7 +876,7 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="3">
+      <c r="A11" s="4">
         <v>42893</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -899,7 +905,7 @@
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="3">
+      <c r="A12" s="4">
         <v>42896</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -928,7 +934,7 @@
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="3">
+      <c r="A13" s="4">
         <v>42903</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -957,7 +963,7 @@
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="3">
+      <c r="A14" s="4">
         <v>42910</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -986,7 +992,7 @@
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="3">
+      <c r="A15" s="4">
         <v>42917</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1015,7 +1021,7 @@
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="3">
+      <c r="A16" s="4">
         <v>42924</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1044,7 +1050,7 @@
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="3">
+      <c r="A17" s="4">
         <v>42931</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1073,7 +1079,7 @@
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="3">
+      <c r="A18" s="4">
         <v>42938</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1102,7 +1108,7 @@
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="3">
+      <c r="A19" s="4">
         <v>42945</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1131,7 +1137,7 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="3">
+      <c r="A20" s="4">
         <v>42952</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1160,7 +1166,7 @@
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="3">
+      <c r="A21" s="4">
         <v>42959</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1189,7 +1195,7 @@
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="3">
+      <c r="A22" s="4">
         <v>42967</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -1218,7 +1224,7 @@
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="3">
+      <c r="A23" s="4">
         <v>42970</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1247,7 +1253,7 @@
       </c>
     </row>
     <row r="24" spans="1:9">
-      <c r="A24" s="3">
+      <c r="A24" s="4">
         <v>42973</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1276,7 +1282,7 @@
       </c>
     </row>
     <row r="25" spans="1:9">
-      <c r="A25" s="3">
+      <c r="A25" s="4">
         <v>42980</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1305,7 +1311,7 @@
       </c>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="3">
+      <c r="A26" s="4">
         <v>42987</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -1334,7 +1340,7 @@
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="3">
+      <c r="A27" s="4">
         <v>42993</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -1363,7 +1369,7 @@
       </c>
     </row>
     <row r="28" spans="1:9">
-      <c r="A28" s="3">
+      <c r="A28" s="4">
         <v>42998</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -1392,7 +1398,7 @@
       </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="3">
+      <c r="A29" s="4">
         <v>43002</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -1421,7 +1427,7 @@
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="3">
+      <c r="A30" s="4">
         <v>43005</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -1450,7 +1456,7 @@
       </c>
     </row>
     <row r="31" spans="1:9">
-      <c r="A31" s="3">
+      <c r="A31" s="4">
         <v>43008</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -1479,7 +1485,7 @@
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="3">
+      <c r="A32" s="4">
         <v>43015</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -1508,7 +1514,7 @@
       </c>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="3">
+      <c r="A33" s="4">
         <v>43022</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -1537,7 +1543,7 @@
       </c>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="3">
+      <c r="A34" s="4">
         <v>43028</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -1566,7 +1572,7 @@
       </c>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="3">
+      <c r="A35" s="4">
         <v>43036</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -1595,7 +1601,7 @@
       </c>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="3">
+      <c r="A36" s="4">
         <v>43043</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -1624,7 +1630,7 @@
       </c>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="3">
+      <c r="A37" s="4">
         <v>43052</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -1653,7 +1659,7 @@
       </c>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="3">
+      <c r="A38" s="4">
         <v>43176</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -1682,7 +1688,7 @@
       </c>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="3">
+      <c r="A39" s="4">
         <v>43190</v>
       </c>
       <c r="B39" s="2" t="s">
@@ -1711,7 +1717,7 @@
       </c>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="3">
+      <c r="A40" s="4">
         <v>43197</v>
       </c>
       <c r="B40" s="2" t="s">
@@ -1740,7 +1746,7 @@
       </c>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="3">
+      <c r="A41" s="4">
         <v>43204</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -1769,7 +1775,7 @@
       </c>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="3">
+      <c r="A42" s="4">
         <v>43211</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -1798,7 +1804,7 @@
       </c>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="3">
+      <c r="A43" s="4">
         <v>43218</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -1827,7 +1833,7 @@
       </c>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="3">
+      <c r="A44" s="4">
         <v>43225</v>
       </c>
       <c r="B44" s="2" t="s">
@@ -1856,7 +1862,7 @@
       </c>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="3">
+      <c r="A45" s="4">
         <v>43233</v>
       </c>
       <c r="B45" s="2" t="s">
@@ -1885,7 +1891,7 @@
       </c>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="3">
+      <c r="A46" s="4">
         <v>43239</v>
       </c>
       <c r="B46" s="2" t="s">
@@ -1914,7 +1920,7 @@
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="3">
+      <c r="A47" s="4">
         <v>43246</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -1943,7 +1949,7 @@
       </c>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="3">
+      <c r="A48" s="4">
         <v>43260</v>
       </c>
       <c r="B48" s="2" t="s">
@@ -1972,7 +1978,7 @@
       </c>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="3">
+      <c r="A49" s="4">
         <v>43267</v>
       </c>
       <c r="B49" s="2" t="s">

</xml_diff>